<commit_message>
Refreshed aggregated and recent data files
Added new data for April and May 2023. Mainly from counties that post data on their websites (SF, Santa Clara, Sacramento, Alameda, Orange, LA, San Diego)
</commit_message>
<xml_diff>
--- a/Recent_Data.xlsx
+++ b/Recent_Data.xlsx
@@ -229,7 +229,7 @@
     <t>San Diego Central Jail, George Bailey Detention Facility, East Mesa Re-Entry Facility, Vista Detention Facility, Las Colinas Detention and Re-Entry Facility, South Bay Detention Facility, and Facility 8 Detention Facility</t>
   </si>
   <si>
-    <t>Intake &amp; Release Center, Jail #2 and Jail #5</t>
+    <t>Intake &amp; Release Center, Jail #2 and Jail #18</t>
   </si>
   <si>
     <t>John J. Zunino Facility, San Joaquin County Honor Farm</t>
@@ -977,7 +977,7 @@
     </row>
     <row r="4" spans="1:38">
       <c r="A4" s="2">
-        <v>44988</v>
+        <v>45044</v>
       </c>
       <c r="B4" t="s">
         <v>38</v>
@@ -986,21 +986,21 @@
         <v>89</v>
       </c>
       <c r="J4">
-        <v>650</v>
+        <v>624</v>
       </c>
       <c r="K4">
-        <v>420</v>
+        <v>584</v>
       </c>
       <c r="L4">
-        <v>35.00269251</v>
+        <v>36.34245778</v>
       </c>
       <c r="M4">
-        <v>22.61712439</v>
+        <v>34.01281305</v>
       </c>
     </row>
     <row r="5" spans="1:38">
       <c r="A5" s="2">
-        <v>44991</v>
+        <v>45047</v>
       </c>
       <c r="B5" t="s">
         <v>38</v>
@@ -1009,28 +1009,28 @@
         <v>89</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>2201</v>
+        <v>2213</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>37430</v>
+        <v>37706</v>
       </c>
       <c r="H5">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>1900</v>
+        <v>1766</v>
       </c>
       <c r="N5">
-        <v>679</v>
+        <v>688</v>
       </c>
       <c r="O5">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:38">
@@ -1810,7 +1810,7 @@
     </row>
     <row r="35" spans="1:36">
       <c r="A35" s="2">
-        <v>44974</v>
+        <v>45048</v>
       </c>
       <c r="B35" t="s">
         <v>52</v>
@@ -1819,13 +1819,13 @@
         <v>103</v>
       </c>
       <c r="D35">
-        <v>72</v>
+        <v>17</v>
       </c>
       <c r="F35">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I35">
-        <v>14253</v>
+        <v>13689</v>
       </c>
     </row>
     <row r="36" spans="1:36">
@@ -2248,7 +2248,7 @@
     </row>
     <row r="50" spans="1:36">
       <c r="A50" s="2">
-        <v>44762</v>
+        <v>44774</v>
       </c>
       <c r="B50" t="s">
         <v>60</v>
@@ -2256,13 +2256,19 @@
       <c r="C50" t="s">
         <v>111</v>
       </c>
-      <c r="E50">
-        <v>1288</v>
+      <c r="N50">
+        <v>474</v>
+      </c>
+      <c r="O50">
+        <v>0</v>
+      </c>
+      <c r="V50">
+        <v>4108</v>
       </c>
     </row>
     <row r="51" spans="1:36">
       <c r="A51" s="2">
-        <v>44774</v>
+        <v>44910</v>
       </c>
       <c r="B51" t="s">
         <v>60</v>
@@ -2270,19 +2276,25 @@
       <c r="C51" t="s">
         <v>111</v>
       </c>
-      <c r="N51">
-        <v>474</v>
-      </c>
-      <c r="O51">
-        <v>0</v>
-      </c>
-      <c r="V51">
-        <v>4108</v>
+      <c r="W51">
+        <v>387</v>
+      </c>
+      <c r="X51">
+        <v>222</v>
+      </c>
+      <c r="Y51">
+        <v>57.36434109</v>
+      </c>
+      <c r="Z51">
+        <v>21.44702842</v>
+      </c>
+      <c r="AE51">
+        <v>83</v>
       </c>
     </row>
     <row r="52" spans="1:36">
       <c r="A52" s="2">
-        <v>44910</v>
+        <v>44991</v>
       </c>
       <c r="B52" t="s">
         <v>60</v>
@@ -2290,25 +2302,13 @@
       <c r="C52" t="s">
         <v>111</v>
       </c>
-      <c r="W52">
-        <v>387</v>
-      </c>
-      <c r="X52">
-        <v>222</v>
-      </c>
-      <c r="Y52">
-        <v>57.36434109</v>
-      </c>
-      <c r="Z52">
-        <v>21.44702842</v>
-      </c>
-      <c r="AE52">
-        <v>83</v>
+      <c r="D52">
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:36">
       <c r="A53" s="2">
-        <v>44991</v>
+        <v>45023</v>
       </c>
       <c r="B53" t="s">
         <v>60</v>
@@ -2316,11 +2316,11 @@
       <c r="C53" t="s">
         <v>111</v>
       </c>
-      <c r="D53">
-        <v>3</v>
+      <c r="E53">
+        <v>1601</v>
       </c>
       <c r="G53">
-        <v>20871</v>
+        <v>21101</v>
       </c>
     </row>
     <row r="54" spans="1:36">
@@ -2621,7 +2621,7 @@
     </row>
     <row r="64" spans="1:36">
       <c r="A64" s="2">
-        <v>44977</v>
+        <v>45047</v>
       </c>
       <c r="B64" t="s">
         <v>63</v>
@@ -2630,16 +2630,16 @@
         <v>114</v>
       </c>
       <c r="D64">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E64">
-        <v>4017</v>
+        <v>4124</v>
       </c>
       <c r="G64">
-        <v>48352</v>
+        <v>51299</v>
       </c>
       <c r="H64">
-        <v>10</v>
+        <v>89</v>
       </c>
     </row>
     <row r="65" spans="1:38">
@@ -2664,7 +2664,7 @@
     </row>
     <row r="66" spans="1:38">
       <c r="A66" s="2">
-        <v>44930</v>
+        <v>44966</v>
       </c>
       <c r="B66" t="s">
         <v>64</v>
@@ -2673,7 +2673,7 @@
         <v>115</v>
       </c>
       <c r="D66">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA66">
         <v>1</v>
@@ -2818,7 +2818,7 @@
     </row>
     <row r="74" spans="1:38">
       <c r="A74" s="2">
-        <v>44986</v>
+        <v>45042</v>
       </c>
       <c r="B74" t="s">
         <v>67</v>
@@ -2827,19 +2827,19 @@
         <v>118</v>
       </c>
       <c r="D74">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="E74">
-        <v>4470</v>
+        <v>4563</v>
       </c>
       <c r="F74">
         <v>3</v>
       </c>
       <c r="G74">
-        <v>58654</v>
+        <v>59379</v>
       </c>
       <c r="I74">
-        <v>2849</v>
+        <v>2994</v>
       </c>
     </row>
     <row r="75" spans="1:38">
@@ -3111,7 +3111,7 @@
     </row>
     <row r="84" spans="1:36">
       <c r="A84" s="2">
-        <v>44994</v>
+        <v>45042</v>
       </c>
       <c r="B84" t="s">
         <v>70</v>
@@ -3120,13 +3120,13 @@
         <v>121</v>
       </c>
       <c r="AA84">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="AB84">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AC84">
-        <v>3394</v>
+        <v>3423</v>
       </c>
     </row>
     <row r="85" spans="1:36">
@@ -3246,7 +3246,7 @@
     </row>
     <row r="90" spans="1:36">
       <c r="A90" s="2">
-        <v>44842</v>
+        <v>44910</v>
       </c>
       <c r="B90" t="s">
         <v>71</v>
@@ -3254,13 +3254,13 @@
       <c r="C90" t="s">
         <v>122</v>
       </c>
-      <c r="G90">
-        <v>43173</v>
+      <c r="AD90">
+        <v>9849</v>
       </c>
     </row>
     <row r="91" spans="1:36">
       <c r="A91" s="2">
-        <v>44910</v>
+        <v>45001</v>
       </c>
       <c r="B91" t="s">
         <v>71</v>
@@ -3268,13 +3268,13 @@
       <c r="C91" t="s">
         <v>122</v>
       </c>
-      <c r="AD91">
-        <v>9849</v>
+      <c r="AA91">
+        <v>4</v>
       </c>
     </row>
     <row r="92" spans="1:36">
       <c r="A92" s="2">
-        <v>44938</v>
+        <v>45034</v>
       </c>
       <c r="B92" t="s">
         <v>71</v>
@@ -3282,16 +3282,16 @@
       <c r="C92" t="s">
         <v>122</v>
       </c>
-      <c r="D92">
-        <v>3</v>
-      </c>
-      <c r="E92">
-        <v>670</v>
+      <c r="W92">
+        <v>966</v>
+      </c>
+      <c r="AC92">
+        <v>648</v>
       </c>
     </row>
     <row r="93" spans="1:36">
       <c r="A93" s="2">
-        <v>44973</v>
+        <v>45038</v>
       </c>
       <c r="B93" t="s">
         <v>71</v>
@@ -3299,19 +3299,13 @@
       <c r="C93" t="s">
         <v>122</v>
       </c>
-      <c r="W93">
-        <v>939</v>
-      </c>
-      <c r="AA93">
-        <v>3</v>
-      </c>
-      <c r="AC93">
-        <v>637</v>
+      <c r="G93">
+        <v>46612</v>
       </c>
     </row>
     <row r="94" spans="1:36">
       <c r="A94" s="2">
-        <v>44974</v>
+        <v>45050</v>
       </c>
       <c r="B94" t="s">
         <v>71</v>
@@ -3319,8 +3313,14 @@
       <c r="C94" t="s">
         <v>122</v>
       </c>
+      <c r="D94">
+        <v>2</v>
+      </c>
+      <c r="E94">
+        <v>694</v>
+      </c>
       <c r="I94">
-        <v>809</v>
+        <v>836</v>
       </c>
     </row>
     <row r="95" spans="1:36">
@@ -3755,7 +3755,7 @@
     </row>
     <row r="112" spans="1:36">
       <c r="A112" s="2">
-        <v>44993</v>
+        <v>45049</v>
       </c>
       <c r="B112" t="s">
         <v>76</v>
@@ -3764,25 +3764,25 @@
         <v>127</v>
       </c>
       <c r="D112">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="E112">
-        <v>2602</v>
+        <v>2793</v>
       </c>
       <c r="G112">
-        <v>87246</v>
+        <v>90871</v>
       </c>
       <c r="I112">
-        <v>2919</v>
+        <v>2935</v>
       </c>
       <c r="AA112">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="AC112">
-        <v>1462</v>
+        <v>1549</v>
       </c>
       <c r="AD112">
-        <v>202853</v>
+        <v>211671</v>
       </c>
     </row>
     <row r="113" spans="1:36">

</xml_diff>